<commit_message>
a lot of mess
</commit_message>
<xml_diff>
--- a/prosseced data/aic_species_list1.csv.xlsx
+++ b/prosseced data/aic_species_list1.csv.xlsx
@@ -9,11 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1275" yWindow="0" windowWidth="19215" windowHeight="8340" activeTab="1"/>
+    <workbookView xWindow="1275" yWindow="0" windowWidth="19215" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="aic_species_list1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="ממוין מודל ומקור" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -3905,8 +3905,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="Q29" sqref="Q29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>

</xml_diff>